<commit_message>
Added DownLoad Issues File test
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>testSuccessfulLogOut</t>
+  </si>
+  <si>
+    <t>testSuccessfulIssuesFileDownLoad</t>
+  </si>
+  <si>
+    <t>downloadPath</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>Richmond County.docx</t>
+  </si>
+  <si>
+    <t>C:\\Users\\jslee\\Downloads</t>
   </si>
 </sst>
 </file>
@@ -430,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,15 +456,15 @@
     <col min="1" max="1" width="44" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -460,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -471,27 +486,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -502,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
@@ -513,40 +528,77 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the download path for Chrome and FireFox
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -49,7 +49,7 @@
     <t>Richmond County.docx</t>
   </si>
   <si>
-    <t>C:\\Users\\jslee\\Downloads</t>
+    <t>C:\\testfolder\\SeleniumDownloads</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
     <col min="1" max="1" width="44" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Update Selenium Standalone to 2.53.0 and update firefox launch options
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>C:\\testfolder\\SeleniumDownloads</t>
+  </si>
+  <si>
+    <t>testSuccessfulIssuesFileDownLoadFiref</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,11 +597,56 @@
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="A16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Download Test_Attachment Test
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>testSuccessfulIssuesFileDownLoadFiref</t>
+  </si>
+  <si>
+    <t>Richmond.docx</t>
+  </si>
+  <si>
+    <t>mp</t>
+  </si>
+  <si>
+    <t>051-0-176-00-0</t>
+  </si>
+  <si>
+    <t>testSuccessfulSumSheetDownLoadFiref</t>
+  </si>
+  <si>
+    <t>Test Attchment.pdf</t>
   </si>
 </sst>
 </file>
@@ -123,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -147,6 +162,7 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,8 +476,8 @@
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" customWidth="1"/>
@@ -613,7 +629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>11</v>
       </c>
@@ -627,26 +643,104 @@
         <v>10</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Download Attachment Firefox in FileViewPage class
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -55,9 +55,6 @@
     <t>testSuccessfulIssuesFileDownLoadFiref</t>
   </si>
   <si>
-    <t>Richmond.docx</t>
-  </si>
-  <si>
     <t>mp</t>
   </si>
   <si>
@@ -67,7 +64,7 @@
     <t>testSuccessfulSumSheetDownLoadFiref</t>
   </si>
   <si>
-    <t>Test Attchment.pdf</t>
+    <t>Richmond Document 123.docx</t>
   </si>
 </sst>
 </file>
@@ -466,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +474,7 @@
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" customWidth="1"/>
@@ -643,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,7 +663,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
@@ -675,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
@@ -686,7 +683,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>2</v>
@@ -695,13 +692,13 @@
         <v>4</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create addAttachment as Admin user and TestSuccessfulAdminAddAttach
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -65,6 +65,39 @@
   </si>
   <si>
     <t>Richmond Document 123.docx</t>
+  </si>
+  <si>
+    <t>documentpath</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>Jason Lee</t>
+  </si>
+  <si>
+    <t>C:\\testfolder\\</t>
+  </si>
+  <si>
+    <t>Richmond County</t>
+  </si>
+  <si>
+    <t>filetitle</t>
+  </si>
+  <si>
+    <t>testSuccessfulAdminAddAttachment</t>
+  </si>
+  <si>
+    <t>addingAttachment</t>
+  </si>
+  <si>
+    <t>152-3-182-00-0</t>
+  </si>
+  <si>
+    <t>Bap1.JPEG</t>
+  </si>
+  <si>
+    <t>rese7</t>
   </si>
 </sst>
 </file>
@@ -461,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>11</v>
       </c>
@@ -643,25 +676,25 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -681,7 +714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>14</v>
       </c>
@@ -701,43 +734,95 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="9"/>
+    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Create New User and CreateNewUser_Test
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>username</t>
   </si>
@@ -79,25 +79,76 @@
     <t>C:\\testfolder\\</t>
   </si>
   <si>
+    <t>filetitle</t>
+  </si>
+  <si>
+    <t>testSuccessfulAdminAddAttachment</t>
+  </si>
+  <si>
+    <t>addingAttachment</t>
+  </si>
+  <si>
+    <t>Bap1.JPEG</t>
+  </si>
+  <si>
+    <t>nusername</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>telenumber</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>confirmpw</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>imgname</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>npassword</t>
+  </si>
+  <si>
+    <t>testSuccessfulNewUserCreate</t>
+  </si>
+  <si>
     <t>Richmond County</t>
   </si>
   <si>
-    <t>filetitle</t>
-  </si>
-  <si>
-    <t>testSuccessfulAdminAddAttachment</t>
-  </si>
-  <si>
-    <t>addingAttachment</t>
-  </si>
-  <si>
-    <t>152-3-182-00-0</t>
-  </si>
-  <si>
-    <t>Bap1.JPEG</t>
-  </si>
-  <si>
-    <t>rese7</t>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>071-4-088-00-0</t>
+  </si>
+  <si>
+    <t>NewClientUser</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>770.330.1111</t>
+  </si>
+  <si>
+    <t>newclient@user2.com</t>
+  </si>
+  <si>
+    <t>clientuser1</t>
+  </si>
+  <si>
+    <t>toshiya3.jpg</t>
   </si>
 </sst>
 </file>
@@ -494,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +561,9 @@
     <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -659,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>11</v>
       </c>
@@ -676,25 +729,25 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -714,7 +767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>14</v>
       </c>
@@ -734,24 +787,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>17</v>
@@ -766,7 +819,7 @@
         <v>12</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>16</v>
@@ -775,38 +828,126 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H28" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -814,8 +955,13 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -823,6 +969,94 @@
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding TestUserCreation_Check DB Fixed admin add attachment and test webtable
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="68">
   <si>
     <t>username</t>
   </si>
@@ -88,9 +88,6 @@
     <t>addingAttachment</t>
   </si>
   <si>
-    <t>Bap1.JPEG</t>
-  </si>
-  <si>
     <t>nusername</t>
   </si>
   <si>
@@ -124,15 +121,9 @@
     <t>testSuccessfulNewUserCreate</t>
   </si>
   <si>
-    <t>Richmond County</t>
-  </si>
-  <si>
     <t>password1</t>
   </si>
   <si>
-    <t>071-4-088-00-0</t>
-  </si>
-  <si>
     <t>NewClientUser</t>
   </si>
   <si>
@@ -149,6 +140,87 @@
   </si>
   <si>
     <t>toshiya3.jpg</t>
+  </si>
+  <si>
+    <t>testSuccessfulNewUserCreationDBcheck</t>
+  </si>
+  <si>
+    <t>NewDataEntryUser</t>
+  </si>
+  <si>
+    <t>NewParaUser1</t>
+  </si>
+  <si>
+    <t>NewAdminUserTest</t>
+  </si>
+  <si>
+    <t>newparauser1@testing.com</t>
+  </si>
+  <si>
+    <t>newadminusertest@testing.com</t>
+  </si>
+  <si>
+    <t>newclientuser@testing.com</t>
+  </si>
+  <si>
+    <t>newdataentryuser@testing.com</t>
+  </si>
+  <si>
+    <t>parauser1</t>
+  </si>
+  <si>
+    <t>adminuser1</t>
+  </si>
+  <si>
+    <t>dataentryuser1</t>
+  </si>
+  <si>
+    <t>770.111.2222</t>
+  </si>
+  <si>
+    <t>404.222.3333</t>
+  </si>
+  <si>
+    <t>678.444.5555</t>
+  </si>
+  <si>
+    <t>770.999.3456</t>
+  </si>
+  <si>
+    <t>Paralegal</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>parauser1.jpg</t>
+  </si>
+  <si>
+    <t>admin1.jpg</t>
+  </si>
+  <si>
+    <t>clientuser1.jpg</t>
+  </si>
+  <si>
+    <t>dataentryuser1.jpg</t>
+  </si>
+  <si>
+    <t>Data Entry</t>
+  </si>
+  <si>
+    <t>City of Decatur 2</t>
+  </si>
+  <si>
+    <t>88-88888-88</t>
+  </si>
+  <si>
+    <t>addingDocument</t>
+  </si>
+  <si>
+    <t>TestCertInput1.xlsx</t>
+  </si>
+  <si>
+    <t>rock1.jpg</t>
   </si>
 </sst>
 </file>
@@ -219,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -244,6 +316,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,10 +633,10 @@
     <col min="5" max="5" width="38.7109375" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="11" width="14.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -589,46 +662,58 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="A3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>1</v>
-      </c>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -642,7 +727,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>0</v>
@@ -650,413 +735,661 @@
       <c r="C11" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="A16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="D20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="E20" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="12" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B31" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D31" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H31" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+    </row>
+    <row r="37" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+    </row>
+    <row r="41" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="E44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J49" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L49" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="C50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F52" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="12" t="s">
+      <c r="G52" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K52" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H28" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="L52" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L31" s="11" t="s">
+      <c r="D53" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H32" t="s">
-        <v>41</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="12" t="s">
+      <c r="F53" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J53" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K53" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L32" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
+      <c r="L53" s="12" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding TestSuccessfulAddAttachment DB check
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="84">
   <si>
     <t>username</t>
   </si>
@@ -221,6 +221,54 @@
   </si>
   <si>
     <t>rock1.jpg</t>
+  </si>
+  <si>
+    <t>City of Decatur 3</t>
+  </si>
+  <si>
+    <t>99-999-999999</t>
+  </si>
+  <si>
+    <t>attachment3</t>
+  </si>
+  <si>
+    <t>attach4</t>
+  </si>
+  <si>
+    <t>gb3.jpg</t>
+  </si>
+  <si>
+    <t>kiar3.jpg</t>
+  </si>
+  <si>
+    <t>testSuccessfulAddAttachmentDBcheck</t>
+  </si>
+  <si>
+    <t>11-675-090898</t>
+  </si>
+  <si>
+    <t>addDocument</t>
+  </si>
+  <si>
+    <t>attachDocument2</t>
+  </si>
+  <si>
+    <t>gb1.jpg</t>
+  </si>
+  <si>
+    <t>golgo13.PNG</t>
+  </si>
+  <si>
+    <t>fcII.jpg</t>
+  </si>
+  <si>
+    <t>addRockman1</t>
+  </si>
+  <si>
+    <t>attachFC2</t>
+  </si>
+  <si>
+    <t>058-2-196-00-0</t>
   </si>
 </sst>
 </file>
@@ -618,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD39"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,24 +1046,56 @@
       </c>
     </row>
     <row r="34" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="A34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="35" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="A35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="36" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
@@ -1038,356 +1118,476 @@
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="A38" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="39" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="A39" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="40" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-    </row>
-    <row r="41" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="A40" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="43" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+    </row>
+    <row r="44" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B47" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C47" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D47" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E47" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F47" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G47" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H47" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="I47" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J43" s="11" t="s">
+      <c r="J47" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="K47" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L43" s="11" t="s">
+      <c r="L47" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="48" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B48" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C48" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D48" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E48" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F48" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="G48" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H48" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="12" t="s">
+      <c r="I48" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="J44" s="12" t="s">
+      <c r="J48" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="K48" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L44" s="12" t="s">
+      <c r="L48" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+    <row r="49" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B53" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C53" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G53" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H53" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I49" s="11" t="s">
+      <c r="I53" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J49" s="11" t="s">
+      <c r="J53" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K49" s="11" t="s">
+      <c r="K53" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L49" s="11" t="s">
+      <c r="L53" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B54" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C54" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D54" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F54" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G54" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H54" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I50" s="12" t="s">
+      <c r="I54" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J50" s="12" t="s">
+      <c r="J54" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="K54" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L50" s="12" t="s">
+      <c r="L54" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B55" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C55" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D55" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E55" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F55" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G55" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H55" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I51" s="12" t="s">
+      <c r="I55" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="J51" s="12" t="s">
+      <c r="J55" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="K51" s="12" t="s">
+      <c r="K55" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L51" s="12" t="s">
+      <c r="L55" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C56" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D56" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E56" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F56" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G52" s="12" t="s">
+      <c r="G56" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H52" s="12" t="s">
+      <c r="H56" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I52" s="12" t="s">
+      <c r="I56" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="J52" s="12" t="s">
+      <c r="J56" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K52" s="12" t="s">
+      <c r="K56" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L52" s="12" t="s">
+      <c r="L56" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B57" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C57" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D57" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E57" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F57" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G53" s="12" t="s">
+      <c r="G57" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H53" s="12" t="s">
+      <c r="H57" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I53" s="12" t="s">
+      <c r="I57" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J53" s="12" t="s">
+      <c r="J57" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K53" s="12" t="s">
+      <c r="K57" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L53" s="12" t="s">
+      <c r="L57" s="12" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created Test Successful Client Creation and Test New Client Check in DB
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="118">
   <si>
     <t>username</t>
   </si>
@@ -208,9 +208,6 @@
     <t>Data Entry</t>
   </si>
   <si>
-    <t>City of Decatur 2</t>
-  </si>
-  <si>
     <t>88-88888-88</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
     <t>rock1.jpg</t>
   </si>
   <si>
-    <t>City of Decatur 3</t>
-  </si>
-  <si>
     <t>99-999-999999</t>
   </si>
   <si>
@@ -269,6 +263,114 @@
   </si>
   <si>
     <t>058-2-196-00-0</t>
+  </si>
+  <si>
+    <t>clientname</t>
+  </si>
+  <si>
+    <t>clientphone</t>
+  </si>
+  <si>
+    <t>clientext</t>
+  </si>
+  <si>
+    <t>clientaddress</t>
+  </si>
+  <si>
+    <t>clientcity</t>
+  </si>
+  <si>
+    <t>clientstate</t>
+  </si>
+  <si>
+    <t>clientzip</t>
+  </si>
+  <si>
+    <t>NewClientTestA</t>
+  </si>
+  <si>
+    <t>770-111-2222</t>
+  </si>
+  <si>
+    <t>2344 New Test Dr.</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>32299</t>
+  </si>
+  <si>
+    <t>NewClientTestB</t>
+  </si>
+  <si>
+    <t>404-33-4444</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>1111 Address St.</t>
+  </si>
+  <si>
+    <t>Marietta</t>
+  </si>
+  <si>
+    <t>30022</t>
+  </si>
+  <si>
+    <t>ClientUserT1</t>
+  </si>
+  <si>
+    <t>ClientUserT2</t>
+  </si>
+  <si>
+    <t>123-111-9999</t>
+  </si>
+  <si>
+    <t>678-990-1234</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>333 Street Dr.</t>
+  </si>
+  <si>
+    <t>888 My Road Dr.</t>
+  </si>
+  <si>
+    <t>Doraville</t>
+  </si>
+  <si>
+    <t>30023</t>
+  </si>
+  <si>
+    <t>Avondale</t>
+  </si>
+  <si>
+    <t>23004</t>
+  </si>
+  <si>
+    <t>testSuccessfulNewClientCreationDBcheck</t>
+  </si>
+  <si>
+    <t>testSuccessfulNewClientCreation</t>
+  </si>
+  <si>
+    <t>NewClientUserA</t>
+  </si>
+  <si>
+    <t>JasonTestClient3</t>
+  </si>
+  <si>
+    <t>JasonTestClient2</t>
   </si>
 </sst>
 </file>
@@ -666,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +1100,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>18</v>
@@ -1007,16 +1109,16 @@
         <v>34</v>
       </c>
       <c r="E32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>65</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1024,7 +1126,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>18</v>
@@ -1033,7 +1135,7 @@
         <v>34</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>22</v>
@@ -1042,7 +1144,7 @@
         <v>19</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1050,7 +1152,7 @@
         <v>21</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>18</v>
@@ -1059,16 +1161,16 @@
         <v>34</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1076,7 +1178,7 @@
         <v>21</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>18</v>
@@ -1085,16 +1187,16 @@
         <v>34</v>
       </c>
       <c r="E35" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1119,7 +1221,7 @@
     </row>
     <row r="38" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>17</v>
@@ -1145,10 +1247,10 @@
     </row>
     <row r="39" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>18</v>
@@ -1157,24 +1259,24 @@
         <v>34</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>18</v>
@@ -1183,24 +1285,24 @@
         <v>34</v>
       </c>
       <c r="E40" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>77</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>18</v>
@@ -1209,24 +1311,24 @@
         <v>34</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>18</v>
@@ -1235,16 +1337,16 @@
         <v>34</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1318,7 +1420,7 @@
         <v>34</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>31</v>
@@ -1589,6 +1691,220 @@
       </c>
       <c r="L57" s="12" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J60" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F61" s="12">
+        <v>123</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J62" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H66" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J66" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J67" s="12" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update AddNewUserTest update RTest
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="375" windowWidth="15405" windowHeight="7590"/>
+    <workbookView xWindow="480" yWindow="435" windowWidth="15405" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseDataSets" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="124">
   <si>
     <t>username</t>
   </si>
@@ -139,48 +139,12 @@
     <t>testSuccessfulNewUserCreationDBcheck</t>
   </si>
   <si>
-    <t>NewDataEntryUser</t>
-  </si>
-  <si>
-    <t>NewParaUser1</t>
-  </si>
-  <si>
     <t>NewAdminUserTest</t>
   </si>
   <si>
-    <t>newparauser1@testing.com</t>
-  </si>
-  <si>
-    <t>newadminusertest@testing.com</t>
-  </si>
-  <si>
-    <t>newclientuser@testing.com</t>
-  </si>
-  <si>
-    <t>newdataentryuser@testing.com</t>
-  </si>
-  <si>
-    <t>parauser1</t>
-  </si>
-  <si>
     <t>adminuser1</t>
   </si>
   <si>
-    <t>dataentryuser1</t>
-  </si>
-  <si>
-    <t>770.111.2222</t>
-  </si>
-  <si>
-    <t>404.222.3333</t>
-  </si>
-  <si>
-    <t>678.444.5555</t>
-  </si>
-  <si>
-    <t>770.999.3456</t>
-  </si>
-  <si>
     <t>Paralegal</t>
   </si>
   <si>
@@ -391,7 +355,40 @@
     <t>NewClientUserA2</t>
   </si>
   <si>
-    <t>clientuserA2</t>
+    <t>NewParaUser2</t>
+  </si>
+  <si>
+    <t>NewAdminUser2</t>
+  </si>
+  <si>
+    <t>NewClientUser2</t>
+  </si>
+  <si>
+    <t>NewDataEntryUser2</t>
+  </si>
+  <si>
+    <t>parauser2@testing.com</t>
+  </si>
+  <si>
+    <t>newadminuser2@testing.com</t>
+  </si>
+  <si>
+    <t>newclientuser2@testing.com</t>
+  </si>
+  <si>
+    <t>newdataentryuser2@testing.com</t>
+  </si>
+  <si>
+    <t>771.111.2222</t>
+  </si>
+  <si>
+    <t>402.222.3333</t>
+  </si>
+  <si>
+    <t>673.444.5555</t>
+  </si>
+  <si>
+    <t>774.999.3456</t>
   </si>
 </sst>
 </file>
@@ -803,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +816,7 @@
     <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.85546875" customWidth="1"/>
     <col min="12" max="12" width="20.28515625" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
@@ -841,10 +838,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -852,10 +849,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -863,10 +860,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -874,10 +871,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,10 +913,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,13 +1067,13 @@
         <v>37</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1090,13 +1087,13 @@
         <v>37</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1138,7 +1135,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>16</v>
@@ -1147,16 +1144,16 @@
         <v>32</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1164,7 +1161,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>16</v>
@@ -1173,7 +1170,7 @@
         <v>32</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>20</v>
@@ -1182,7 +1179,7 @@
         <v>17</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1190,7 +1187,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>16</v>
@@ -1199,16 +1196,16 @@
         <v>32</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1216,7 +1213,7 @@
         <v>19</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>16</v>
@@ -1225,16 +1222,16 @@
         <v>32</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1259,7 +1256,7 @@
     </row>
     <row r="37" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>15</v>
@@ -1285,10 +1282,10 @@
     </row>
     <row r="38" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>16</v>
@@ -1297,24 +1294,24 @@
         <v>32</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>16</v>
@@ -1323,24 +1320,24 @@
         <v>32</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>16</v>
@@ -1349,24 +1346,24 @@
         <v>32</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>16</v>
@@ -1375,16 +1372,16 @@
         <v>32</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1461,7 +1458,7 @@
         <v>32</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>29</v>
@@ -1470,7 +1467,7 @@
         <v>34</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>35</v>
@@ -1479,10 +1476,10 @@
         <v>36</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>124</v>
+        <v>32</v>
       </c>
       <c r="L47" s="12" t="s">
         <v>17</v>
@@ -1491,20 +1488,46 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M48" s="12" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
@@ -1600,34 +1623,34 @@
         <v>32</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="E53" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H53" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="H53" s="12" t="s">
-        <v>50</v>
-      </c>
       <c r="I53" s="12" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="J53" s="12" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="L53" s="12" t="s">
         <v>17</v>
       </c>
       <c r="M53" s="12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -1641,34 +1664,34 @@
         <v>32</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="J54" s="12" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="L54" s="12" t="s">
         <v>17</v>
       </c>
       <c r="M54" s="12" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -1682,112 +1705,106 @@
         <v>32</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>88</v>
+        <v>43</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="L55" s="12" t="s">
         <v>17</v>
       </c>
       <c r="M55" s="12" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" s="12" t="s">
+      <c r="I56" s="9"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J58" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="H56" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J56" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="L56" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M56" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I59" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J59" s="11" t="s">
-        <v>82</v>
+      <c r="C59" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" s="12">
+        <v>123</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>16</v>
@@ -1796,58 +1813,37 @@
         <v>32</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F60" s="12">
-        <v>123</v>
+        <v>77</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F61" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="H61" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I61" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>93</v>
-      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
@@ -1861,197 +1857,186 @@
       <c r="J62" s="9"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
+      <c r="A63" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J64" s="11" t="s">
+      <c r="A64" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>82</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J64" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J65" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G69" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="H65" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="I65" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J65" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H66" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="I66" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J66" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E69" s="1" t="s">
+      <c r="H69" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>111</v>
+      <c r="I69" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>88</v>
+        <v>100</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G70" s="15" t="s">
-        <v>119</v>
+        <v>101</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="F71" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G71" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H71" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="I71" s="13" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the data provider excel sheet
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="115">
   <si>
     <t>username</t>
   </si>
@@ -265,106 +265,103 @@
     <t>4562</t>
   </si>
   <si>
-    <t>Import7.6A.xlsx</t>
-  </si>
-  <si>
-    <t>7.6.11A</t>
-  </si>
-  <si>
-    <t>7.6.11B</t>
-  </si>
-  <si>
-    <t>Import7.6B.xlsx</t>
-  </si>
-  <si>
-    <t>7.6.112A</t>
-  </si>
-  <si>
-    <t>7.6.112B</t>
-  </si>
-  <si>
-    <t>Client7.6A</t>
-  </si>
-  <si>
-    <t>Client7.6B2</t>
-  </si>
-  <si>
-    <t>Client7.6A2</t>
-  </si>
-  <si>
-    <t>Client7.6D2</t>
-  </si>
-  <si>
-    <t>Client7.6C2</t>
-  </si>
-  <si>
-    <t>NewAdminUserD</t>
-  </si>
-  <si>
-    <t>NewParaUserD</t>
-  </si>
-  <si>
-    <t>NewDataEntryUserD</t>
-  </si>
-  <si>
-    <t>NewClientUserD</t>
-  </si>
-  <si>
-    <t>1234 Street Dr.</t>
-  </si>
-  <si>
-    <t>1878 My Road Dr.</t>
-  </si>
-  <si>
-    <t>2213 Address St.</t>
-  </si>
-  <si>
-    <t>4578 New Test Dr.</t>
-  </si>
-  <si>
-    <t>404-111-2222</t>
-  </si>
-  <si>
-    <t>678-33-4444</t>
-  </si>
-  <si>
-    <t>779-111-9999</t>
-  </si>
-  <si>
-    <t>123-990-1234</t>
-  </si>
-  <si>
-    <t>newadminuserb4@testing.com</t>
-  </si>
-  <si>
-    <t>parauserb4@testing.com</t>
-  </si>
-  <si>
-    <t>newdataentryuserb4@testing.com</t>
-  </si>
-  <si>
-    <t>newclient4@userb.com</t>
-  </si>
-  <si>
-    <t>addDocument4</t>
-  </si>
-  <si>
-    <t>attachDocument4</t>
-  </si>
-  <si>
-    <t>addRockman4</t>
-  </si>
-  <si>
-    <t>attachment32</t>
-  </si>
-  <si>
-    <t>attach42</t>
-  </si>
-  <si>
-    <t>addingAttachment2</t>
-  </si>
-  <si>
-    <t>addingDocument2</t>
+    <t>7.6.16004</t>
+  </si>
+  <si>
+    <t>7.6.16003</t>
+  </si>
+  <si>
+    <t>7.6.16002</t>
+  </si>
+  <si>
+    <t>7.6.16001</t>
+  </si>
+  <si>
+    <t>Import7.6C.xlsx</t>
+  </si>
+  <si>
+    <t>Import7.6D.xlsx</t>
+  </si>
+  <si>
+    <t>404-111-2220</t>
+  </si>
+  <si>
+    <t>678-33-4440</t>
+  </si>
+  <si>
+    <t>779-111-9990</t>
+  </si>
+  <si>
+    <t>123-990-1230</t>
+  </si>
+  <si>
+    <t>200 H St.</t>
+  </si>
+  <si>
+    <t>400 Dog Town Dr.</t>
+  </si>
+  <si>
+    <t>1899 Small Road Dr.</t>
+  </si>
+  <si>
+    <t>1222 H Street Dr.</t>
+  </si>
+  <si>
+    <t>Client7.6.16B</t>
+  </si>
+  <si>
+    <t>Client7.6.16A</t>
+  </si>
+  <si>
+    <t>Client7.6.16D</t>
+  </si>
+  <si>
+    <t>Client7.6.16C</t>
+  </si>
+  <si>
+    <t>NewParaUserD0</t>
+  </si>
+  <si>
+    <t>NewAdminUserD0</t>
+  </si>
+  <si>
+    <t>NewDataEntryUserD0</t>
+  </si>
+  <si>
+    <t>NewClientUserD0</t>
+  </si>
+  <si>
+    <t>newclientAA@user.com</t>
+  </si>
+  <si>
+    <t>newdataentryuserAA@testing.com</t>
+  </si>
+  <si>
+    <t>parauserAA@testing.com</t>
+  </si>
+  <si>
+    <t>newadminuserAA@testing.com</t>
+  </si>
+  <si>
+    <t>addingAttach4</t>
+  </si>
+  <si>
+    <t>attachDoc4</t>
+  </si>
+  <si>
+    <t>addRock4</t>
+  </si>
+  <si>
+    <t>attaching1</t>
+  </si>
+  <si>
+    <t>attach001</t>
+  </si>
+  <si>
+    <t>addingAttach22</t>
+  </si>
+  <si>
+    <t>addingDocCCC</t>
   </si>
 </sst>
 </file>
@@ -388,7 +385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +401,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -474,7 +477,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,7 +786,7 @@
   <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,8 +820,8 @@
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>94</v>
+      <c r="B2" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>31</v>
@@ -824,8 +831,8 @@
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>93</v>
+      <c r="B3" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>31</v>
@@ -835,8 +842,8 @@
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>96</v>
+      <c r="B4" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>31</v>
@@ -846,8 +853,8 @@
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>95</v>
+      <c r="B5" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>31</v>
@@ -878,8 +885,8 @@
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>96</v>
+      <c r="B9" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>31</v>
@@ -1007,13 +1014,13 @@
       <c r="A21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>96</v>
+      <c r="B21" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="18" t="s">
         <v>83</v>
       </c>
       <c r="E21" s="12" t="s">
@@ -1061,8 +1068,8 @@
       <c r="A25" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>91</v>
+      <c r="B25" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>16</v>
@@ -1070,11 +1077,11 @@
       <c r="D25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>115</v>
+      <c r="E25" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>17</v>
@@ -1087,8 +1094,8 @@
       <c r="A26" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>91</v>
+      <c r="B26" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>16</v>
@@ -1096,11 +1103,11 @@
       <c r="D26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>114</v>
+      <c r="E26" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>17</v>
@@ -1113,8 +1120,8 @@
       <c r="A27" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>91</v>
+      <c r="B27" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>16</v>
@@ -1122,10 +1129,10 @@
       <c r="D27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="12" t="s">
+      <c r="E27" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>112</v>
       </c>
       <c r="G27" s="12" t="s">
@@ -1139,8 +1146,8 @@
       <c r="A28" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>91</v>
+      <c r="B28" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>16</v>
@@ -1148,11 +1155,11 @@
       <c r="D28" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>113</v>
+      <c r="E28" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>17</v>
@@ -1211,8 +1218,8 @@
       <c r="A32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>91</v>
+      <c r="B32" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>16</v>
@@ -1220,11 +1227,11 @@
       <c r="D32" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>109</v>
+      <c r="E32" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>108</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>17</v>
@@ -1237,8 +1244,8 @@
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>90</v>
+      <c r="B33" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>16</v>
@@ -1246,11 +1253,11 @@
       <c r="D33" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>110</v>
+      <c r="F33" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>17</v>
@@ -1263,8 +1270,8 @@
       <c r="A34" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>90</v>
+      <c r="B34" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>16</v>
@@ -1272,11 +1279,11 @@
       <c r="D34" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>111</v>
+      <c r="E34" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>17</v>
@@ -1358,8 +1365,8 @@
       <c r="C40" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>96</v>
+      <c r="D40" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>28</v>
@@ -1367,14 +1374,14 @@
       <c r="F40" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="12" t="s">
-        <v>88</v>
+      <c r="G40" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>108</v>
+      <c r="I40" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>31</v>
@@ -1399,8 +1406,8 @@
       <c r="C41" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>95</v>
+      <c r="D41" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>28</v>
@@ -1408,14 +1415,14 @@
       <c r="F41" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G41" s="15" t="s">
         <v>76</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="I41" s="9" t="s">
-        <v>107</v>
+      <c r="I41" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>31</v>
@@ -1523,8 +1530,8 @@
       <c r="C46" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>94</v>
+      <c r="D46" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>28</v>
@@ -1538,7 +1545,7 @@
       <c r="H46" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="19" t="s">
         <v>106</v>
       </c>
       <c r="J46" s="12" t="s">
@@ -1564,8 +1571,8 @@
       <c r="C47" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>93</v>
+      <c r="D47" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>28</v>
@@ -1579,8 +1586,8 @@
       <c r="H47" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="I47" s="9" t="s">
-        <v>105</v>
+      <c r="I47" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>31</v>
@@ -1643,17 +1650,17 @@
       <c r="C51" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>101</v>
+      <c r="D51" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G51" s="12" t="s">
-        <v>100</v>
+      <c r="G51" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="H51" s="12" t="s">
         <v>56</v>
@@ -1675,17 +1682,17 @@
       <c r="C52" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>102</v>
+      <c r="D52" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G52" s="12" t="s">
-        <v>99</v>
+      <c r="G52" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="H52" s="12" t="s">
         <v>59</v>
@@ -1761,17 +1768,17 @@
       <c r="C56" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G56" s="12" t="s">
-        <v>97</v>
+      <c r="G56" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>63</v>
@@ -1793,17 +1800,17 @@
       <c r="C57" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D57" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>104</v>
+      <c r="D57" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G57" s="12" t="s">
-        <v>98</v>
+      <c r="G57" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>65</v>
@@ -1857,8 +1864,8 @@
       <c r="C61" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D61" s="12" t="s">
-        <v>91</v>
+      <c r="D61" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="E61" s="13" t="s">
         <v>70</v>
@@ -1866,14 +1873,14 @@
       <c r="F61" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G61" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="I61" s="13" t="s">
+      <c r="G61" s="17" t="s">
         <v>87</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -1886,8 +1893,8 @@
       <c r="C62" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D62" s="12" t="s">
-        <v>90</v>
+      <c r="D62" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="E62" s="13" t="s">
         <v>75</v>
@@ -1895,13 +1902,13 @@
       <c r="F62" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G62" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H62" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I62" s="13" t="s">
+      <c r="G62" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I62" s="18" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated Rtest and created newAdminCreateTest
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="120">
   <si>
     <t>username</t>
   </si>
@@ -362,6 +362,21 @@
   </si>
   <si>
     <t>addingDocCCC</t>
+  </si>
+  <si>
+    <t>testSuccessfulNewAdminUserCreationDBcheck</t>
+  </si>
+  <si>
+    <t>sysadmin</t>
+  </si>
+  <si>
+    <t>777.123.2222</t>
+  </si>
+  <si>
+    <t>jasonadmin@admintesting.com</t>
+  </si>
+  <si>
+    <t>money.jpg</t>
   </si>
 </sst>
 </file>
@@ -783,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,106 +820,156 @@
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B6" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="C6" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B7" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="C7" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B8" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="C8" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B9" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>103</v>
-      </c>
       <c r="C9" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>0</v>
@@ -912,47 +977,31 @@
       <c r="C12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>0</v>
@@ -969,7 +1018,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>2</v>
@@ -985,49 +1034,51 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>103</v>
+      <c r="A21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>83</v>
+        <v>4</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1035,188 +1086,162 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H28" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B29" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C29" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="18" t="s">
+      <c r="D29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F29" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G29" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="H29" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B30" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="18" t="s">
+      <c r="D30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F30" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G30" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="H30" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B31" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="18" t="s">
+      <c r="D31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F31" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G31" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H31" s="12" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>99</v>
@@ -1228,421 +1253,414 @@
         <v>31</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+    <row r="37" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B37" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="18" t="s">
+      <c r="D37" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F37" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G37" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H37" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="38" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B38" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="18" t="s">
+      <c r="D38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F38" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G38" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H38" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-    </row>
-    <row r="36" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-    </row>
-    <row r="37" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+    </row>
+    <row r="41" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C43" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E43" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F43" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G43" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H43" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="11" t="s">
+      <c r="I43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="11" t="s">
+      <c r="J43" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K39" s="11" t="s">
+      <c r="K43" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="11" t="s">
+      <c r="L43" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M39" s="11" t="s">
+      <c r="M43" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+    <row r="44" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="16" t="s">
+      <c r="C44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E44" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F44" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="16" t="s">
+      <c r="G44" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="H40" s="12" t="s">
+      <c r="H44" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I44" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="J40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L40" s="12" t="s">
+      <c r="J44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L44" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M40" s="12" t="s">
+      <c r="M44" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="16" t="s">
+      <c r="C45" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E45" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F45" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G45" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H45" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="I41" s="19" t="s">
+      <c r="I45" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="J41" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L41" s="12" t="s">
+      <c r="J45" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L45" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M41" s="12" t="s">
+      <c r="M45" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B49" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C49" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E49" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F49" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="G49" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="H49" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I45" s="11" t="s">
+      <c r="I49" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="11" t="s">
+      <c r="J49" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="K49" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L45" s="11" t="s">
+      <c r="L49" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M45" s="11" t="s">
+      <c r="M49" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="16" t="s">
+      <c r="C50" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G50" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H46" s="12" t="s">
+      <c r="H50" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I46" s="19" t="s">
+      <c r="I50" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J46" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L46" s="12" t="s">
+      <c r="J50" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L50" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="M46" s="12" t="s">
+      <c r="M50" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H47" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I47" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M47" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>16</v>
@@ -1651,116 +1669,109 @@
         <v>31</v>
       </c>
       <c r="D51" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E55" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F55" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G51" s="16" t="s">
+      <c r="G55" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H55" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I51" s="12" t="s">
+      <c r="I55" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J51" s="12" t="s">
+      <c r="J55" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G55" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>16</v>
@@ -1769,146 +1780,232 @@
         <v>31</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I56" s="12" t="s">
         <v>57</v>
       </c>
       <c r="J56" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J59" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G60" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J60" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B61" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="I57" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J57" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F58" s="9"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D61" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F62" s="9"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E65" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F65" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G61" s="17" t="s">
+      <c r="G65" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="H61" s="18" t="s">
+      <c r="H65" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="I61" s="18" t="s">
+      <c r="I65" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B66" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" s="16" t="s">
+      <c r="C66" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="E66" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F66" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G62" s="18" t="s">
+      <c r="G66" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H62" s="18" t="s">
+      <c r="H66" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="I62" s="18" t="s">
+      <c r="I66" s="18" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating add Sales Date test
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated Add Sale Date test
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="134">
   <si>
     <t>username</t>
   </si>
@@ -415,19 +415,10 @@
     <t>day12</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>testSuccessfulAddSaleDates</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -851,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="D57" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,7 +2053,7 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>0</v>
@@ -2109,7 +2100,7 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>116</v>
@@ -2118,13 +2109,13 @@
         <v>4</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G70" s="12" t="s">
         <v>133</v>
@@ -2136,22 +2127,22 @@
         <v>133</v>
       </c>
       <c r="J70" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L70" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M70" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N70" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="O70" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating RTest to include new add sales date test
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -67,9 +67,6 @@
     <t>client</t>
   </si>
   <si>
-    <t>Jason Lee</t>
-  </si>
-  <si>
     <t>C:\\testfolder\\</t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t>batchdate</t>
   </si>
   <si>
-    <t>Nov 28 2016</t>
-  </si>
-  <si>
     <t>mapparcelnumber1</t>
   </si>
   <si>
@@ -244,9 +238,6 @@
     <t>C:\\testfolder\\uploadfiles\\</t>
   </si>
   <si>
-    <t>Dec 28 2016</t>
-  </si>
-  <si>
     <t>nothing</t>
   </si>
   <si>
@@ -265,105 +256,6 @@
     <t>4562</t>
   </si>
   <si>
-    <t>7.6.16004</t>
-  </si>
-  <si>
-    <t>7.6.16003</t>
-  </si>
-  <si>
-    <t>7.6.16002</t>
-  </si>
-  <si>
-    <t>7.6.16001</t>
-  </si>
-  <si>
-    <t>Import7.6C.xlsx</t>
-  </si>
-  <si>
-    <t>Import7.6D.xlsx</t>
-  </si>
-  <si>
-    <t>404-111-2220</t>
-  </si>
-  <si>
-    <t>678-33-4440</t>
-  </si>
-  <si>
-    <t>779-111-9990</t>
-  </si>
-  <si>
-    <t>123-990-1230</t>
-  </si>
-  <si>
-    <t>200 H St.</t>
-  </si>
-  <si>
-    <t>400 Dog Town Dr.</t>
-  </si>
-  <si>
-    <t>1899 Small Road Dr.</t>
-  </si>
-  <si>
-    <t>1222 H Street Dr.</t>
-  </si>
-  <si>
-    <t>Client7.6.16B</t>
-  </si>
-  <si>
-    <t>Client7.6.16A</t>
-  </si>
-  <si>
-    <t>Client7.6.16D</t>
-  </si>
-  <si>
-    <t>Client7.6.16C</t>
-  </si>
-  <si>
-    <t>NewParaUserD0</t>
-  </si>
-  <si>
-    <t>NewAdminUserD0</t>
-  </si>
-  <si>
-    <t>NewDataEntryUserD0</t>
-  </si>
-  <si>
-    <t>NewClientUserD0</t>
-  </si>
-  <si>
-    <t>newclientAA@user.com</t>
-  </si>
-  <si>
-    <t>newdataentryuserAA@testing.com</t>
-  </si>
-  <si>
-    <t>parauserAA@testing.com</t>
-  </si>
-  <si>
-    <t>newadminuserAA@testing.com</t>
-  </si>
-  <si>
-    <t>addingAttach4</t>
-  </si>
-  <si>
-    <t>attachDoc4</t>
-  </si>
-  <si>
-    <t>addRock4</t>
-  </si>
-  <si>
-    <t>attaching1</t>
-  </si>
-  <si>
-    <t>attach001</t>
-  </si>
-  <si>
-    <t>addingAttach22</t>
-  </si>
-  <si>
-    <t>addingDocCCC</t>
-  </si>
-  <si>
     <t>testSuccessfulNewAdminUserCreationDBcheck</t>
   </si>
   <si>
@@ -373,9 +265,6 @@
     <t>777.123.2222</t>
   </si>
   <si>
-    <t>jasonadmin@admintesting.com</t>
-  </si>
-  <si>
     <t>money.jpg</t>
   </si>
   <si>
@@ -419,6 +308,117 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>Dec 20 2016</t>
+  </si>
+  <si>
+    <t>Nov 20 2016</t>
+  </si>
+  <si>
+    <t>Json Lee</t>
+  </si>
+  <si>
+    <t>jsonadmin2@admintesting.com</t>
+  </si>
+  <si>
+    <t>NewParaUserD1</t>
+  </si>
+  <si>
+    <t>NewAdminUserD1</t>
+  </si>
+  <si>
+    <t>NewClientUserD1</t>
+  </si>
+  <si>
+    <t>NewDataEntryUserD1</t>
+  </si>
+  <si>
+    <t>newadminuserd1@testing.com</t>
+  </si>
+  <si>
+    <t>parauserd1@testing.com</t>
+  </si>
+  <si>
+    <t>Client7.18.16C</t>
+  </si>
+  <si>
+    <t>Client7.18.16D</t>
+  </si>
+  <si>
+    <t>Client7.18.16A</t>
+  </si>
+  <si>
+    <t>Client7.18.16B</t>
+  </si>
+  <si>
+    <t>401-111-2220</t>
+  </si>
+  <si>
+    <t>671-33-4440</t>
+  </si>
+  <si>
+    <t>771-111-9990</t>
+  </si>
+  <si>
+    <t>121-990-1230</t>
+  </si>
+  <si>
+    <t>4010 Dog Town Dr.</t>
+  </si>
+  <si>
+    <t>2010 H St.</t>
+  </si>
+  <si>
+    <t>1120 H Street Dr.</t>
+  </si>
+  <si>
+    <t>1180 Small Road Dr.</t>
+  </si>
+  <si>
+    <t>7.18.16003</t>
+  </si>
+  <si>
+    <t>7.18.16001</t>
+  </si>
+  <si>
+    <t>addingDoc7.18</t>
+  </si>
+  <si>
+    <t>addingAttach7.18</t>
+  </si>
+  <si>
+    <t>attach7.18</t>
+  </si>
+  <si>
+    <t>attaching7.18</t>
+  </si>
+  <si>
+    <t>7.18.16004</t>
+  </si>
+  <si>
+    <t>7.18.16002</t>
+  </si>
+  <si>
+    <t>Import7.18D.xlsx</t>
+  </si>
+  <si>
+    <t>Import7.18C.xlsx</t>
+  </si>
+  <si>
+    <t>attachDocument7.18</t>
+  </si>
+  <si>
+    <t>addingAttachm7.18</t>
+  </si>
+  <si>
+    <t>addRockman7.18</t>
+  </si>
+  <si>
+    <t>newclientD1@user.com</t>
+  </si>
+  <si>
+    <t>newdataentryuserD1@testing.com</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,6 +464,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -539,6 +545,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D57" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +873,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -873,76 +882,82 @@
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="M2" s="12" t="s">
-        <v>119</v>
-      </c>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -954,16 +969,17 @@
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -971,10 +987,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -985,7 +1001,7 @@
         <v>103</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -993,10 +1009,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1028,7 +1044,7 @@
         <v>103</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1157,16 +1173,16 @@
         <v>103</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1179,7 +1195,7 @@
     <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>15</v>
@@ -1194,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>14</v>
@@ -1205,106 +1221,106 @@
     </row>
     <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="D29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="H29" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="D30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="H30" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="D31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="H31" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="D32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="H32" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1329,7 +1345,7 @@
     </row>
     <row r="35" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>15</v>
@@ -1344,7 +1360,7 @@
         <v>12</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>14</v>
@@ -1355,80 +1371,80 @@
     </row>
     <row r="36" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C37" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="H37" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C38" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="H38" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1455,7 +1471,7 @@
     <row r="42" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>0</v>
@@ -1464,116 +1480,116 @@
         <v>1</v>
       </c>
       <c r="D43" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="F43" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="G43" s="11" t="s">
         <v>15</v>
       </c>
       <c r="H43" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="J43" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K43" s="11" t="s">
+      <c r="L43" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L43" s="11" t="s">
+      <c r="M43" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="M43" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>103</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H44" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H44" s="12" t="s">
+      <c r="I44" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M44" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="I44" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="I45" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="M45" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -1620,7 +1636,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>0</v>
@@ -1629,116 +1645,116 @@
         <v>1</v>
       </c>
       <c r="D49" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="F49" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="G49" s="11" t="s">
         <v>15</v>
       </c>
       <c r="H49" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I49" s="11" t="s">
+      <c r="J49" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J49" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K49" s="11" t="s">
+      <c r="L49" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L49" s="11" t="s">
+      <c r="M49" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="M49" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>36</v>
-      </c>
       <c r="G50" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>106</v>
       </c>
       <c r="J50" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K50" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L50" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M50" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L51" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H51" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="J51" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="M51" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -1749,7 +1765,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>0</v>
@@ -1758,89 +1774,89 @@
         <v>1</v>
       </c>
       <c r="D54" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="F54" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="G54" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="H54" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="I54" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I54" s="11" t="s">
+      <c r="J54" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="H55" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I55" s="12" t="s">
+      <c r="J55" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="J55" s="12" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="H56" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J56" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J56" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -1867,7 +1883,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>0</v>
@@ -1876,89 +1892,89 @@
         <v>1</v>
       </c>
       <c r="D59" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="F59" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="G59" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="H59" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="I59" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I59" s="11" t="s">
+      <c r="J59" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="J59" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="H60" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J60" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J60" s="12" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="H61" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J61" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="I61" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J61" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -1966,7 +1982,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>0</v>
@@ -1975,85 +1991,85 @@
         <v>1</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>70</v>
+        <v>110</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>75</v>
+        <v>107</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>0</v>
@@ -2062,87 +2078,87 @@
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="F70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="J70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="L70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="M70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="N70" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="O70" s="12" t="s">
-        <v>133</v>
+      <c r="D70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="L70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N70" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="O70" s="22" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Including sendmail helper utility and email test-output emailable report
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -514,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -533,9 +533,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -548,6 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O76"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,153 +876,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="12" t="s">
+      <c r="J2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="C6" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="C7" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="C8" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="C9" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
@@ -1026,31 +1031,31 @@
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -1058,45 +1063,43 @@
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -1106,505 +1109,498 @@
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E22" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="18" t="s">
+      <c r="C26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G29" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H29" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="18" t="s">
+      <c r="D30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F30" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G30" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H30" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="18" t="s">
+      <c r="D31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F31" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G31" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="H31" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="18" t="s">
+      <c r="D32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F32" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G32" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H32" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+    <row r="33" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C33" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="18" t="s">
+      <c r="D33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F33" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G33" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="H33" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-    </row>
     <row r="34" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G36" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H36" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+    <row r="37" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C37" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="18" t="s">
+      <c r="D37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F37" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G37" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="H37" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+    <row r="38" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B38" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C38" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="18" t="s">
+      <c r="D38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F38" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G38" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="12" t="s">
+      <c r="H38" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+    <row r="39" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="18" t="s">
+      <c r="D39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F39" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="G39" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="12" t="s">
+      <c r="H39" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-    </row>
     <row r="40" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-    </row>
-    <row r="41" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+    </row>
     <row r="42" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+    <row r="43" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D44" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E44" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F44" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G44" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H44" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="I44" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J43" s="11" t="s">
+      <c r="J44" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="K44" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L43" s="11" t="s">
+      <c r="L44" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M43" s="11" t="s">
+      <c r="M44" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="45" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B45" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="16" t="s">
+      <c r="C45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E45" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F45" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="G45" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="H44" s="12" t="s">
+      <c r="H45" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I44" s="19" t="s">
+      <c r="I45" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J44" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L44" s="12" t="s">
+      <c r="J45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L45" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M44" s="12" t="s">
+      <c r="M45" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B46" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="16" t="s">
+      <c r="C46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E46" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F46" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G46" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="H46" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I45" s="19" t="s">
+      <c r="I46" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J45" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L45" s="12" t="s">
+      <c r="J46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L46" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M45" s="12" t="s">
+      <c r="M46" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
@@ -1635,240 +1631,243 @@
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C50" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D50" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E50" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F50" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G50" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H50" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I49" s="11" t="s">
+      <c r="I50" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J49" s="11" t="s">
+      <c r="J50" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K49" s="11" t="s">
+      <c r="K50" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L49" s="11" t="s">
+      <c r="L50" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M49" s="11" t="s">
+      <c r="M50" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="16" t="s">
+      <c r="C51" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E51" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F51" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G51" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H51" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="I50" s="19" t="s">
+      <c r="I51" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J50" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L50" s="12" t="s">
+      <c r="J51" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K51" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L51" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M50" s="12" t="s">
+      <c r="M51" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="16" t="s">
+      <c r="C52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F52" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G52" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H52" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="I51" s="19" t="s">
+      <c r="I52" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="J51" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L51" s="12" t="s">
+      <c r="J52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L52" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M51" s="12" t="s">
+      <c r="M52" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C55" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D55" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E55" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F55" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G55" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H55" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I54" s="11" t="s">
+      <c r="I55" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J54" s="11" t="s">
+      <c r="J55" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D55" s="16" t="s">
+      <c r="C56" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E56" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F56" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G55" s="16" t="s">
+      <c r="G56" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="H55" s="12" t="s">
+      <c r="H56" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I55" s="12" t="s">
+      <c r="I56" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J55" s="12" t="s">
+      <c r="J56" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B57" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="16" t="s">
+      <c r="C57" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E57" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F57" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G56" s="16" t="s">
+      <c r="G57" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="H57" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I56" s="12" t="s">
+      <c r="I57" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J56" s="12" t="s">
+      <c r="J57" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
@@ -1882,164 +1881,146 @@
       <c r="J58" s="9"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B60" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C60" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D60" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E60" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F60" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G60" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="H60" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I59" s="11" t="s">
+      <c r="I60" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J59" s="11" t="s">
+      <c r="J60" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B61" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C60" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D60" s="16" t="s">
+      <c r="C61" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E61" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F61" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G60" s="16" t="s">
+      <c r="G61" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H60" s="12" t="s">
+      <c r="H61" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I60" s="12" t="s">
+      <c r="I61" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J60" s="12" t="s">
+      <c r="J61" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B62" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D61" s="16" t="s">
+      <c r="C62" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E62" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F62" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G61" s="16" t="s">
+      <c r="G62" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H61" s="12" t="s">
+      <c r="H62" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I61" s="12" t="s">
+      <c r="I62" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J61" s="12" t="s">
+      <c r="J62" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F62" s="9"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F63" s="9"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F65" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="H65" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="I65" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E65" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F65" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G65" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I65" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -2048,134 +2029,147 @@
       <c r="C66" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H66" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I66" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E66" s="21" t="s">
+      <c r="E67" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F66" s="13" t="s">
+      <c r="F67" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G66" s="18" t="s">
+      <c r="G67" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="H66" s="18" t="s">
+      <c r="H67" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="I66" s="18" t="s">
+      <c r="I67" s="17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H70" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="I70" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="J70" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="K70" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L69" s="1" t="s">
+      <c r="L70" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M69" s="1" t="s">
+      <c r="M70" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N69" s="1" t="s">
+      <c r="N70" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O69" s="1" t="s">
+      <c r="O70" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B71" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="C71" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D70" s="22" t="s">
+      <c r="D71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E70" s="22" t="s">
+      <c r="E71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="F70" s="22" t="s">
+      <c r="F71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="G70" s="22" t="s">
+      <c r="G71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="H70" s="22" t="s">
+      <c r="H71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="I70" s="22" t="s">
+      <c r="I71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="J70" s="22" t="s">
+      <c r="J71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="K70" s="22" t="s">
+      <c r="K71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="L70" s="22" t="s">
+      <c r="L71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="M70" s="22" t="s">
+      <c r="M71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="N70" s="22" t="s">
+      <c r="N71" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="O70" s="22" t="s">
+      <c r="O71" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
-      <c r="L71" s="9"/>
-      <c r="M71" s="9"/>
-      <c r="N71" s="9"/>
-      <c r="O71" s="9"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B72" s="9"/>
@@ -2256,6 +2250,22 @@
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
       <c r="O76" s="9"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+      <c r="O77" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Included Ant sendMail and updated sendMail in TestBase class
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="137">
   <si>
     <t>username</t>
   </si>
@@ -307,118 +307,127 @@
     <t>testSuccessfulAddSaleDates</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Dec 20 2016</t>
-  </si>
-  <si>
-    <t>Nov 20 2016</t>
-  </si>
-  <si>
     <t>Json Lee</t>
   </si>
   <si>
-    <t>jsonadmin2@admintesting.com</t>
-  </si>
-  <si>
-    <t>NewParaUserD1</t>
-  </si>
-  <si>
-    <t>NewAdminUserD1</t>
-  </si>
-  <si>
-    <t>NewClientUserD1</t>
-  </si>
-  <si>
-    <t>NewDataEntryUserD1</t>
-  </si>
-  <si>
-    <t>newadminuserd1@testing.com</t>
-  </si>
-  <si>
-    <t>parauserd1@testing.com</t>
-  </si>
-  <si>
-    <t>Client7.18.16C</t>
-  </si>
-  <si>
-    <t>Client7.18.16D</t>
-  </si>
-  <si>
-    <t>Client7.18.16A</t>
-  </si>
-  <si>
-    <t>Client7.18.16B</t>
-  </si>
-  <si>
-    <t>401-111-2220</t>
-  </si>
-  <si>
-    <t>671-33-4440</t>
-  </si>
-  <si>
-    <t>771-111-9990</t>
-  </si>
-  <si>
-    <t>121-990-1230</t>
-  </si>
-  <si>
-    <t>4010 Dog Town Dr.</t>
-  </si>
-  <si>
-    <t>2010 H St.</t>
-  </si>
-  <si>
-    <t>1120 H Street Dr.</t>
-  </si>
-  <si>
-    <t>1180 Small Road Dr.</t>
-  </si>
-  <si>
-    <t>7.18.16003</t>
-  </si>
-  <si>
-    <t>7.18.16001</t>
-  </si>
-  <si>
-    <t>addingDoc7.18</t>
-  </si>
-  <si>
-    <t>addingAttach7.18</t>
-  </si>
-  <si>
-    <t>attach7.18</t>
-  </si>
-  <si>
-    <t>attaching7.18</t>
-  </si>
-  <si>
-    <t>7.18.16004</t>
-  </si>
-  <si>
-    <t>7.18.16002</t>
-  </si>
-  <si>
-    <t>Import7.18D.xlsx</t>
-  </si>
-  <si>
-    <t>Import7.18C.xlsx</t>
-  </si>
-  <si>
-    <t>attachDocument7.18</t>
-  </si>
-  <si>
-    <t>addingAttachm7.18</t>
-  </si>
-  <si>
-    <t>addRockman7.18</t>
-  </si>
-  <si>
-    <t>newclientD1@user.com</t>
-  </si>
-  <si>
-    <t>newdataentryuserD1@testing.com</t>
+    <t>NewParaUserD2</t>
+  </si>
+  <si>
+    <t>NewAdminUserD2</t>
+  </si>
+  <si>
+    <t>112022 H Street Dr.</t>
+  </si>
+  <si>
+    <t>118022 Small Road Dr.</t>
+  </si>
+  <si>
+    <t>Jn Lee</t>
+  </si>
+  <si>
+    <t>jnadmin3@admintesting.com</t>
+  </si>
+  <si>
+    <t>NewParaUserD3</t>
+  </si>
+  <si>
+    <t>NewAdminUserD3</t>
+  </si>
+  <si>
+    <t>NewClientUserD3</t>
+  </si>
+  <si>
+    <t>NewDataEntryUserD3</t>
+  </si>
+  <si>
+    <t>7.20b.16003</t>
+  </si>
+  <si>
+    <t>Client7.20b.16C</t>
+  </si>
+  <si>
+    <t>7.20b.16001</t>
+  </si>
+  <si>
+    <t>addingDoc7.20b</t>
+  </si>
+  <si>
+    <t>addingAttach7.20b</t>
+  </si>
+  <si>
+    <t>attach7.20b</t>
+  </si>
+  <si>
+    <t>attaching7.20b</t>
+  </si>
+  <si>
+    <t>Client7.20b.16B</t>
+  </si>
+  <si>
+    <t>7.20b.16002</t>
+  </si>
+  <si>
+    <t>7.20b.16004</t>
+  </si>
+  <si>
+    <t>addingAttachm7.20b</t>
+  </si>
+  <si>
+    <t>attachDocument7.20b</t>
+  </si>
+  <si>
+    <t>addRockman7.20b</t>
+  </si>
+  <si>
+    <t>newclientD3@user.com</t>
+  </si>
+  <si>
+    <t>newdataentryuserD3@testing.com</t>
+  </si>
+  <si>
+    <t>parauserd3@testing.com</t>
+  </si>
+  <si>
+    <t>newadminuserd3@testing.com</t>
+  </si>
+  <si>
+    <t>Client7.20b.16D</t>
+  </si>
+  <si>
+    <t>401-118-2220</t>
+  </si>
+  <si>
+    <t>671-328-4440</t>
+  </si>
+  <si>
+    <t>8 Dog Town Dr.</t>
+  </si>
+  <si>
+    <t>82 H St.</t>
+  </si>
+  <si>
+    <t>771-311-9900</t>
+  </si>
+  <si>
+    <t>121-790-1030</t>
+  </si>
+  <si>
+    <t>Client7.20b.16A</t>
+  </si>
+  <si>
+    <t>Import7.20bD.xlsx</t>
+  </si>
+  <si>
+    <t>Import7.20bC.xlsx</t>
+  </si>
+  <si>
+    <t>Nov 18 2016</t>
+  </si>
+  <si>
+    <t>Dec 18 2016</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -855,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +878,7 @@
     <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.5703125" customWidth="1"/>
     <col min="10" max="11" width="14.85546875" customWidth="1"/>
     <col min="12" max="12" width="20.28515625" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
@@ -927,7 +936,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>27</v>
@@ -942,7 +951,7 @@
         <v>81</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>30</v>
@@ -981,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>30</v>
@@ -992,7 +1001,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>30</v>
@@ -1003,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>30</v>
@@ -1014,7 +1023,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>30</v>
@@ -1051,7 +1060,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>30</v>
@@ -1180,13 +1189,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>10</v>
@@ -1234,19 +1243,19 @@
         <v>18</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>16</v>
@@ -1260,19 +1269,19 @@
         <v>18</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>16</v>
@@ -1286,19 +1295,19 @@
         <v>18</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>16</v>
@@ -1312,19 +1321,19 @@
         <v>18</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>16</v>
@@ -1384,19 +1393,19 @@
         <v>45</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>16</v>
@@ -1410,19 +1419,19 @@
         <v>45</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>16</v>
@@ -1436,19 +1445,19 @@
         <v>45</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>16</v>
@@ -1524,14 +1533,14 @@
       <c r="A45" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>99</v>
+      <c r="B45" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>27</v>
@@ -1540,13 +1549,13 @@
         <v>31</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H45" s="11" t="s">
         <v>32</v>
       </c>
       <c r="I45" s="18" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="J45" s="11" t="s">
         <v>30</v>
@@ -1565,14 +1574,14 @@
       <c r="A46" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>99</v>
+      <c r="B46" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>27</v>
@@ -1587,7 +1596,7 @@
         <v>76</v>
       </c>
       <c r="I46" s="18" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="J46" s="11" t="s">
         <v>30</v>
@@ -1689,14 +1698,14 @@
       <c r="A51" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="11" t="s">
-        <v>99</v>
+      <c r="B51" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>27</v>
@@ -1711,7 +1720,7 @@
         <v>74</v>
       </c>
       <c r="I51" s="18" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="J51" s="11" t="s">
         <v>30</v>
@@ -1730,14 +1739,14 @@
       <c r="A52" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>99</v>
+      <c r="B52" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>27</v>
@@ -1752,7 +1761,7 @@
         <v>75</v>
       </c>
       <c r="I52" s="18" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="J52" s="11" t="s">
         <v>30</v>
@@ -1809,23 +1818,23 @@
       <c r="A56" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="11" t="s">
-        <v>99</v>
+      <c r="B56" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>77</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="H56" s="11" t="s">
         <v>55</v>
@@ -1841,23 +1850,23 @@
       <c r="A57" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="11" t="s">
-        <v>99</v>
+      <c r="B57" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>78</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="H57" s="11" t="s">
         <v>58</v>
@@ -1927,23 +1936,23 @@
       <c r="A61" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>99</v>
+      <c r="B61" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>60</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="H61" s="11" t="s">
         <v>62</v>
@@ -1959,23 +1968,23 @@
       <c r="A62" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>99</v>
+      <c r="B62" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="F62" s="11" t="s">
         <v>61</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="H62" s="11" t="s">
         <v>64</v>
@@ -2023,58 +2032,58 @@
       <c r="A66" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="12" t="s">
-        <v>99</v>
+      <c r="B66" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>72</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="H66" s="17" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="I66" s="17" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>99</v>
+      <c r="B67" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>72</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H67" s="17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -2135,40 +2144,40 @@
         <v>4</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="G71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="H71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="I71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="J71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="K71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="L71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="M71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="N71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="O71" s="21" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>